<commit_message>
Update example XLS(X) files to be based on column name
</commit_message>
<xml_diff>
--- a/examples/custom_layouts/simple_oca.xlsx
+++ b/examples/custom_layouts/simple_oca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -767,25 +767,46 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">OL: Conditional [Condition]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Conditional [Dependencies]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Cardinality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Conformance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Attribute Mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Entry Code Mapping</t>
+    <t xml:space="preserve">CB-CL: Classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB-AN: Attribute Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB-AT: Attribute Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB-FA: Flagged Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CH: Character Encoding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-FT: Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-EC: Entry Codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CC: Conditional [Condition]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CD: Conditional [Dependencies]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CR: Cardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CN: Conformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-UT: Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-AM: Attribute Mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-EM: Entry Code Mapping</t>
   </si>
   <si>
     <t xml:space="preserve">attribute1</t>
@@ -812,10 +833,19 @@
     <t xml:space="preserve">Claim </t>
   </si>
   <si>
-    <t xml:space="preserve">OL: Meta [Form Name]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Meta [Form Description]</t>
+    <t xml:space="preserve">OL-MN: Meta [Form Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-MD: Meta [Form Description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-LA: Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-EN: Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-IN: Information</t>
   </si>
   <si>
     <t xml:space="preserve">Simple OCA</t>
@@ -845,7 +875,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]DDDD&quot;, &quot;MMMM\ DD&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="21">
@@ -1898,14 +1928,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <dxfs count="50">
     <dxf>
@@ -2483,9 +2513,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>119880</xdr:colOff>
+      <xdr:colOff>119520</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2498,13 +2528,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4060800" y="282240"/>
-          <a:ext cx="2900520" cy="820800"/>
+          <a:off x="4061160" y="282600"/>
+          <a:ext cx="2899800" cy="820080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2515,25 +2545,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D59"/>
+  <dimension ref="B1:D973"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="91.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3925,162 +3955,262 @@
     <mergeCell ref="B58:D58"/>
   </mergeCells>
   <conditionalFormatting sqref="F24:F43 C45:C46">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="0"/>
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F43 C45:C46">
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="1"/>
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F43 C45:C46">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="2"/>
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="2">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56 C59:C973 C45:C46">
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="3"/>
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="3">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C45)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56 C59:C973">
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="4"/>
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="4">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C56)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56 C59:C973">
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="5"/>
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="5">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C56)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56 C59:C973">
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="6"/>
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="6">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C56)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="7"/>
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="7">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C44)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="8"/>
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="8">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C44)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="9"/>
+    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="9">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C44)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="10"/>
+    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="10">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C44)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="11"/>
+    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="11">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C27)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="12"/>
+    <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="12">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C27)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="13"/>
+    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="13">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C27)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="14"/>
+    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="14">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C27)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C30">
-    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="15"/>
+    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="15">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C30">
-    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="16"/>
+    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="16">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C30">
-    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="17"/>
+    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="17">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C30">
-    <cfRule type="containsText" priority="20" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="18"/>
+    <cfRule type="containsText" priority="20" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="18">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="containsText" priority="21" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="19"/>
+    <cfRule type="containsText" priority="21" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="19">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="containsText" priority="22" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="20"/>
+    <cfRule type="containsText" priority="22" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="20">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="21"/>
+    <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="21">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="22"/>
+    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="22">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" priority="25" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="23"/>
+    <cfRule type="containsText" priority="25" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="23">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C33)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" priority="26" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="24"/>
+    <cfRule type="containsText" priority="26" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="24">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C33)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="25"/>
+    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="25">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C33)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="26"/>
+    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="26">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C33)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" priority="29" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="27"/>
+    <cfRule type="containsText" priority="29" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="27">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C34)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="28"/>
+    <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="28">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C34)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="29"/>
+    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="29">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C34)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" priority="32" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="30"/>
+    <cfRule type="containsText" priority="32" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="30">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C34)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" priority="33" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="31"/>
+    <cfRule type="containsText" priority="33" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="31">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C35)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" priority="34" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="32"/>
+    <cfRule type="containsText" priority="34" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="32">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C35)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" priority="35" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="33"/>
+    <cfRule type="containsText" priority="35" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="33">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C35)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" priority="36" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="34"/>
+    <cfRule type="containsText" priority="36" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="34">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C35)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C43 C24">
-    <cfRule type="containsText" priority="37" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="35"/>
+    <cfRule type="containsText" priority="37" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="35">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C43 C24">
-    <cfRule type="containsText" priority="38" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="36"/>
+    <cfRule type="containsText" priority="38" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="36">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C43 C24">
-    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="37"/>
+    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="37">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20 C36:C43 C24">
-    <cfRule type="containsText" priority="40" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="38"/>
+    <cfRule type="containsText" priority="40" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="38">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C19)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="containsText" priority="41" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="39"/>
+    <cfRule type="containsText" priority="41" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="39">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C19)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="40"/>
+    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="40">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C19)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="containsText" priority="43" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="41"/>
+    <cfRule type="containsText" priority="43" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="41">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C19)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="44" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="42"/>
+    <cfRule type="containsText" priority="44" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="42">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="45" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="43"/>
+    <cfRule type="containsText" priority="45" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="43">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="46" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="44"/>
+    <cfRule type="containsText" priority="46" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="44">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="47" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="45"/>
+    <cfRule type="containsText" priority="47" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="45">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="48" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="46"/>
+    <cfRule type="containsText" priority="48" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="46">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="49" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="47"/>
+    <cfRule type="containsText" priority="49" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="47">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="50" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="48"/>
+    <cfRule type="containsText" priority="50" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="48">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="51" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="49"/>
+    <cfRule type="containsText" priority="51" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="49">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1" display="paul.knowles@humancolossus.org"/>
     <hyperlink ref="B57" r:id="rId2" display="© The Human Colossus Foundation 2022. Some rights reserved. This work is available under the CC BY-NC-SA 3.0 IGO licence."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4090,17 +4220,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="16.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="19.83"/>
@@ -4113,10 +4243,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="47" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4151,59 +4279,59 @@
     </row>
     <row r="3" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="58" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="G3" s="61" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="H3" s="62" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="I3" s="62" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="J3" s="62" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="K3" s="62" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="L3" s="62" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="M3" s="62" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="N3" s="62" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" s="71" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="63"/>
       <c r="B4" s="64" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C4" s="65" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="66"/>
       <c r="E4" s="67" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F4" s="68"/>
       <c r="G4" s="69"/>
@@ -4215,14 +4343,14 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="73"/>
       <c r="B5" s="74" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D5" s="76"/>
       <c r="E5" s="77" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F5" s="78"/>
       <c r="G5" s="79"/>
@@ -4233,16 +4361,16 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="73"/>
       <c r="B6" s="74" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C6" s="75" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E6" s="77" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F6" s="78"/>
       <c r="G6" s="74"/>
@@ -4456,8 +4584,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4466,17 +4594,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="85" width="22.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="34.83"/>
@@ -4490,7 +4618,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="94.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="95.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="75.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4499,10 +4626,10 @@
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
       <c r="E1" s="89" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F1" s="90" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4511,80 +4638,80 @@
       <c r="C2" s="92"/>
       <c r="D2" s="55"/>
       <c r="E2" s="58" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F2" s="93" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="94" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B3" s="94" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="E3" s="89" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="F3" s="90" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="95" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C4" s="97" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D4" s="98" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E4" s="99"/>
       <c r="F4" s="98" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="95" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B5" s="96" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C5" s="97" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D5" s="98" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E5" s="100"/>
       <c r="F5" s="73" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="95" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B6" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="97" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="97" t="s">
-        <v>91</v>
-      </c>
       <c r="D6" s="98" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E6" s="100"/>
       <c r="F6" s="73"/>
@@ -4727,8 +4854,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>